<commit_message>
Commit on 30 Nov
</commit_message>
<xml_diff>
--- a/src/test/resources/Daily Report(Automated)_ApprovalCall&Position_ SimplVisibility_Sheet.xlsx
+++ b/src/test/resources/Daily Report(Automated)_ApprovalCall&Position_ SimplVisibility_Sheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="47">
   <si>
     <t>Mechant</t>
   </si>
@@ -729,8 +729,8 @@
       <c r="J4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="K4" t="n" s="0">
-        <v>1.0</v>
+      <c r="K4" t="s" s="0">
+        <v>37</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
Tachyon Code Push 20/01/23
</commit_message>
<xml_diff>
--- a/src/test/resources/Daily Report(Automated)_ApprovalCall&Position_ SimplVisibility_Sheet.xlsx
+++ b/src/test/resources/Daily Report(Automated)_ApprovalCall&Position_ SimplVisibility_Sheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="48">
   <si>
     <t>Mechant</t>
   </si>
@@ -797,7 +797,7 @@
         <v>14</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7">

</xml_diff>